<commit_message>
Data of hydrogen-bonded self-healing polyurethane
Data
</commit_message>
<xml_diff>
--- a/Data/Raw data.xlsx
+++ b/Data/Raw data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\番茄\聚氨酯与机器学习\ML投稿\CSV data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8938FF-4923-448C-BA9D-012AD453D8F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD5B718-D235-46FE-B5E8-D31B12ECA843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00AAE7D3-B735-40AF-B5E8-F41082C92CA6}"/>
+    <workbookView xWindow="0" yWindow="2020" windowWidth="25600" windowHeight="13260" xr2:uid="{00AAE7D3-B735-40AF-B5E8-F41082C92CA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t>MOCA-PDM-IPDI-PTEMG-2000-IPDI-PDM-MOCA</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -49,10 +49,6 @@
   </si>
   <si>
     <t>BDO-AHMP-PEG1000-IPDI-PPG3000(tir-OH)-AHMP-BDO</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.88:8.65:2.31:37.5(PEG1000:AHMP:PPG3000:IPDI)</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -481,7 +477,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -529,15 +525,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -854,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{521912C5-85CD-4A9E-A24D-75F7E59E94FF}">
-  <dimension ref="A1:H111"/>
+  <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -868,28 +855,27 @@
     <col min="4" max="4" width="9.25" style="9" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" style="1"/>
     <col min="6" max="6" width="10" style="10" customWidth="1"/>
-    <col min="7" max="7" width="43.25" style="18" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" style="17"/>
+    <col min="7" max="7" width="43.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.5" x14ac:dyDescent="0.3">
       <c r="B1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="E1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -912,7 +898,7 @@
         <v>43.6</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -962,7 +948,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>2</v>
@@ -977,7 +963,7 @@
         <v>100</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1078,13 +1064,13 @@
         <v>25</v>
       </c>
       <c r="E13" s="3">
-        <v>0.5</v>
+        <v>0.17</v>
       </c>
       <c r="F13" s="4">
-        <v>38.4</v>
+        <v>28.1</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1095,10 +1081,10 @@
         <v>25</v>
       </c>
       <c r="E14" s="3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F14" s="4">
-        <v>43.3</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1109,10 +1095,10 @@
         <v>25</v>
       </c>
       <c r="E15" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" s="4">
-        <v>50.2</v>
+        <v>55.5</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1126,7 +1112,7 @@
         <v>6</v>
       </c>
       <c r="F16" s="4">
-        <v>65.3</v>
+        <v>78.099999999999994</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -1140,7 +1126,7 @@
         <v>12</v>
       </c>
       <c r="F17" s="4">
-        <v>73.5</v>
+        <v>82.7</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -1154,7 +1140,7 @@
         <v>24</v>
       </c>
       <c r="F18" s="4">
-        <v>85.4</v>
+        <v>96.7</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1171,13 +1157,13 @@
         <v>25</v>
       </c>
       <c r="E19" s="3">
-        <v>0.17</v>
+        <v>0.5</v>
       </c>
       <c r="F19" s="4">
-        <v>28.1</v>
+        <v>12.4</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1188,10 +1174,10 @@
         <v>25</v>
       </c>
       <c r="E20" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F20" s="4">
-        <v>50</v>
+        <v>17.2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1202,10 +1188,10 @@
         <v>25</v>
       </c>
       <c r="E21" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F21" s="4">
-        <v>55.5</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1216,10 +1202,10 @@
         <v>25</v>
       </c>
       <c r="E22" s="3">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F22" s="4">
-        <v>78.099999999999994</v>
+        <v>53.5</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1230,47 +1216,47 @@
         <v>25</v>
       </c>
       <c r="E23" s="3">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F23" s="4">
-        <v>82.7</v>
+        <v>68.2</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="12"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="8"/>
+      <c r="A24" s="11">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="D24" s="2">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="E24" s="3">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="F24" s="4">
-        <v>96.7</v>
+        <v>56</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="11">
-        <v>5</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="A25" s="12"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="8"/>
       <c r="D25" s="2">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="E25" s="3">
-        <v>0.5</v>
+        <v>4</v>
       </c>
       <c r="F25" s="4">
-        <v>12.4</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1278,13 +1264,13 @@
       <c r="B26" s="7"/>
       <c r="C26" s="8"/>
       <c r="D26" s="2">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="E26" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F26" s="4">
-        <v>17.2</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1292,13 +1278,13 @@
       <c r="B27" s="7"/>
       <c r="C27" s="8"/>
       <c r="D27" s="2">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="E27" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F27" s="4">
-        <v>49</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1306,13 +1292,13 @@
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
       <c r="D28" s="2">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E28" s="3">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F28" s="4">
-        <v>53.5</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1320,50 +1306,50 @@
       <c r="B29" s="7"/>
       <c r="C29" s="8"/>
       <c r="D29" s="2">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E29" s="3">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="F29" s="4">
-        <v>68.2</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="11">
+      <c r="A30" s="12"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="2">
+        <v>60</v>
+      </c>
+      <c r="E30" s="3">
         <v>6</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="6" t="s">
+      <c r="F30" s="4">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="A31" s="11">
+        <v>6</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="2">
-        <v>80</v>
-      </c>
-      <c r="E30" s="3">
-        <v>2</v>
-      </c>
-      <c r="F30" s="4">
-        <v>56</v>
-      </c>
-      <c r="G30" s="9" t="s">
+      <c r="C31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="2">
+        <v>100</v>
+      </c>
+      <c r="E31" s="3">
+        <v>6</v>
+      </c>
+      <c r="F31" s="4">
+        <v>33.4</v>
+      </c>
+      <c r="G31" s="9" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="12"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="2">
-        <v>80</v>
-      </c>
-      <c r="E31" s="3">
-        <v>4</v>
-      </c>
-      <c r="F31" s="4">
-        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -1371,13 +1357,13 @@
       <c r="B32" s="7"/>
       <c r="C32" s="8"/>
       <c r="D32" s="2">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E32" s="3">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F32" s="4">
-        <v>76</v>
+        <v>61.1</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -1388,10 +1374,10 @@
         <v>80</v>
       </c>
       <c r="E33" s="3">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="F33" s="4">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -1399,13 +1385,13 @@
       <c r="B34" s="7"/>
       <c r="C34" s="8"/>
       <c r="D34" s="2">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E34" s="3">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="F34" s="4">
-        <v>39</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -1416,10 +1402,10 @@
         <v>40</v>
       </c>
       <c r="E35" s="3">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="F35" s="4">
-        <v>56</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -1427,13 +1413,13 @@
       <c r="B36" s="7"/>
       <c r="C36" s="8"/>
       <c r="D36" s="2">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="E36" s="3">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="F36" s="4">
-        <v>68</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="14.5" x14ac:dyDescent="0.3">
@@ -1441,7 +1427,7 @@
         <v>7</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>10</v>
@@ -1453,10 +1439,10 @@
         <v>6</v>
       </c>
       <c r="F37" s="4">
-        <v>33.4</v>
+        <v>58</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -1470,7 +1456,7 @@
         <v>12</v>
       </c>
       <c r="F38" s="4">
-        <v>61.1</v>
+        <v>71.900000000000006</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -1478,27 +1464,36 @@
       <c r="B39" s="7"/>
       <c r="C39" s="8"/>
       <c r="D39" s="2">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E39" s="3">
         <v>24</v>
       </c>
       <c r="F39" s="4">
-        <v>89</v>
+        <v>82.8</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="12"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="8"/>
+      <c r="A40" s="11">
+        <v>8</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="D40" s="2">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E40" s="3">
-        <v>24</v>
+        <v>0.25</v>
       </c>
       <c r="F40" s="4">
-        <v>60</v>
+        <v>79</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -1506,13 +1501,13 @@
       <c r="B41" s="7"/>
       <c r="C41" s="8"/>
       <c r="D41" s="2">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E41" s="3">
-        <v>24</v>
+        <v>0.5</v>
       </c>
       <c r="F41" s="4">
-        <v>25</v>
+        <v>83.9</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -1520,36 +1515,27 @@
       <c r="B42" s="7"/>
       <c r="C42" s="8"/>
       <c r="D42" s="2">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="E42" s="3">
-        <v>24</v>
+        <v>0.75</v>
       </c>
       <c r="F42" s="4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="14.5" x14ac:dyDescent="0.3">
-      <c r="A43" s="11">
-        <v>8</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>11</v>
-      </c>
+        <v>86.1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="12"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="8"/>
       <c r="D43" s="2">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="E43" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F43" s="4">
-        <v>58</v>
-      </c>
-      <c r="G43" s="9" t="s">
-        <v>38</v>
+        <v>88.6</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -1557,13 +1543,13 @@
       <c r="B44" s="7"/>
       <c r="C44" s="8"/>
       <c r="D44" s="2">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="E44" s="3">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F44" s="4">
-        <v>71.900000000000006</v>
+        <v>8.4</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -1571,36 +1557,27 @@
       <c r="B45" s="7"/>
       <c r="C45" s="8"/>
       <c r="D45" s="2">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="E45" s="3">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="F45" s="4">
-        <v>82.8</v>
+        <v>24.6</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="11">
-        <v>9</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A46" s="12"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="8"/>
       <c r="D46" s="2">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="E46" s="3">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="F46" s="4">
-        <v>79</v>
-      </c>
-      <c r="G46" s="9" t="s">
-        <v>39</v>
+        <v>91.4</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -1608,13 +1585,13 @@
       <c r="B47" s="7"/>
       <c r="C47" s="8"/>
       <c r="D47" s="2">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="E47" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F47" s="4">
-        <v>83.9</v>
+        <v>94.9</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -1625,24 +1602,33 @@
         <v>45</v>
       </c>
       <c r="E48" s="3">
-        <v>0.75</v>
+        <v>2</v>
       </c>
       <c r="F48" s="4">
-        <v>86.1</v>
+        <v>89.8</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="12"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="8"/>
+      <c r="A49" s="11">
+        <v>9</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="D49" s="2">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="E49" s="3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F49" s="4">
-        <v>88.6</v>
+        <v>54.7</v>
+      </c>
+      <c r="G49" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
@@ -1650,13 +1636,13 @@
       <c r="B50" s="7"/>
       <c r="C50" s="8"/>
       <c r="D50" s="2">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="E50" s="3">
         <v>1</v>
       </c>
       <c r="F50" s="4">
-        <v>8.4</v>
+        <v>68.8</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
@@ -1664,13 +1650,13 @@
       <c r="B51" s="7"/>
       <c r="C51" s="8"/>
       <c r="D51" s="2">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="E51" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F51" s="4">
-        <v>24.6</v>
+        <v>84.1</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
@@ -1678,13 +1664,13 @@
       <c r="B52" s="7"/>
       <c r="C52" s="8"/>
       <c r="D52" s="2">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="E52" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F52" s="4">
-        <v>91.4</v>
+        <v>93.9</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -1692,13 +1678,13 @@
       <c r="B53" s="7"/>
       <c r="C53" s="8"/>
       <c r="D53" s="2">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="E53" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F53" s="4">
-        <v>94.9</v>
+        <v>95.6</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
@@ -1706,36 +1692,27 @@
       <c r="B54" s="7"/>
       <c r="C54" s="8"/>
       <c r="D54" s="2">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="E54" s="3">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F54" s="4">
-        <v>89.8</v>
+        <v>98.9</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="11">
-        <v>10</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>18</v>
-      </c>
+      <c r="A55" s="12"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="8"/>
       <c r="D55" s="2">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E55" s="3">
-        <v>0.5</v>
+        <v>12</v>
       </c>
       <c r="F55" s="4">
-        <v>54.7</v>
-      </c>
-      <c r="G55" s="18" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
@@ -1743,13 +1720,13 @@
       <c r="B56" s="7"/>
       <c r="C56" s="8"/>
       <c r="D56" s="2">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="E56" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F56" s="4">
-        <v>68.8</v>
+        <v>72.099999999999994</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
@@ -1757,13 +1734,13 @@
       <c r="B57" s="7"/>
       <c r="C57" s="8"/>
       <c r="D57" s="2">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="E57" s="3">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F57" s="4">
-        <v>84.1</v>
+        <v>60.3</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -1771,27 +1748,36 @@
       <c r="B58" s="7"/>
       <c r="C58" s="8"/>
       <c r="D58" s="2">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="E58" s="3">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F58" s="4">
-        <v>93.9</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="12"/>
-      <c r="B59" s="7"/>
-      <c r="C59" s="8"/>
+        <v>24.7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="A59" s="11">
+        <v>10</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="D59" s="2">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="E59" s="3">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F59" s="4">
-        <v>95.6</v>
+        <v>42.4</v>
+      </c>
+      <c r="G59" s="9" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
@@ -1799,13 +1785,13 @@
       <c r="B60" s="7"/>
       <c r="C60" s="8"/>
       <c r="D60" s="2">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="E60" s="3">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F60" s="4">
-        <v>98.9</v>
+        <v>67.400000000000006</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
@@ -1813,13 +1799,13 @@
       <c r="B61" s="7"/>
       <c r="C61" s="8"/>
       <c r="D61" s="2">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="E61" s="3">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="F61" s="4">
-        <v>90</v>
+        <v>80.5</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
@@ -1827,64 +1813,64 @@
       <c r="B62" s="7"/>
       <c r="C62" s="8"/>
       <c r="D62" s="2">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="E62" s="3">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="F62" s="4">
-        <v>72.099999999999994</v>
+        <v>97.6</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="12"/>
-      <c r="B63" s="7"/>
-      <c r="C63" s="8"/>
+      <c r="A63" s="11">
+        <v>11</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="D63" s="2">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="E63" s="3">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F63" s="4">
-        <v>60.3</v>
+        <v>14</v>
+      </c>
+      <c r="G63" s="9" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="12"/>
       <c r="B64" s="7"/>
-      <c r="C64" s="8"/>
+      <c r="C64" s="7"/>
       <c r="D64" s="2">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="E64" s="3">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F64" s="4">
-        <v>24.7</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="14.5" x14ac:dyDescent="0.3">
-      <c r="A65" s="11">
-        <v>11</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>24</v>
-      </c>
+        <v>20.7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" s="12"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="8"/>
       <c r="D65" s="2">
-        <v>25</v>
+        <v>140</v>
       </c>
       <c r="E65" s="3">
         <v>12</v>
       </c>
       <c r="F65" s="4">
-        <v>42.4</v>
-      </c>
-      <c r="G65" s="9" t="s">
-        <v>41</v>
+        <v>55.5</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -1892,27 +1878,36 @@
       <c r="B66" s="7"/>
       <c r="C66" s="8"/>
       <c r="D66" s="2">
-        <v>25</v>
+        <v>140</v>
       </c>
       <c r="E66" s="3">
         <v>24</v>
       </c>
       <c r="F66" s="4">
-        <v>67.400000000000006</v>
+        <v>76.8</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="12"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="8"/>
+      <c r="A67" s="11">
+        <v>12</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="D67" s="2">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="E67" s="3">
-        <v>32</v>
+        <v>0.25</v>
       </c>
       <c r="F67" s="4">
-        <v>80.5</v>
+        <v>55.6</v>
+      </c>
+      <c r="G67" s="9" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -1920,50 +1915,41 @@
       <c r="B68" s="7"/>
       <c r="C68" s="8"/>
       <c r="D68" s="2">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="E68" s="3">
-        <v>48</v>
+        <v>0.5</v>
       </c>
       <c r="F68" s="4">
-        <v>97.6</v>
+        <v>75.2</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" s="11">
-        <v>12</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="A69" s="12"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="8"/>
       <c r="D69" s="2">
-        <v>140</v>
+        <v>45</v>
       </c>
       <c r="E69" s="3">
-        <v>3</v>
+        <v>0.75</v>
       </c>
       <c r="F69" s="4">
-        <v>14</v>
-      </c>
-      <c r="G69" s="9" t="s">
-        <v>41</v>
+        <v>80.400000000000006</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="12"/>
       <c r="B70" s="7"/>
-      <c r="C70" s="7"/>
+      <c r="C70" s="8"/>
       <c r="D70" s="2">
-        <v>140</v>
+        <v>45</v>
       </c>
       <c r="E70" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F70" s="4">
-        <v>20.7</v>
+        <v>85.3</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -1971,13 +1957,13 @@
       <c r="B71" s="7"/>
       <c r="C71" s="8"/>
       <c r="D71" s="2">
-        <v>140</v>
+        <v>25</v>
       </c>
       <c r="E71" s="3">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F71" s="4">
-        <v>55.5</v>
+        <v>44.3</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -1985,36 +1971,27 @@
       <c r="B72" s="7"/>
       <c r="C72" s="8"/>
       <c r="D72" s="2">
-        <v>140</v>
+        <v>35</v>
       </c>
       <c r="E72" s="3">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="F72" s="4">
-        <v>76.8</v>
+        <v>84.9</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" s="11">
-        <v>13</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="A73" s="12"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="8"/>
       <c r="D73" s="2">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="E73" s="3">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="F73" s="4">
-        <v>55.6</v>
-      </c>
-      <c r="G73" s="9" t="s">
-        <v>39</v>
+        <v>90.8</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -2022,13 +1999,13 @@
       <c r="B74" s="7"/>
       <c r="C74" s="8"/>
       <c r="D74" s="2">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="E74" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F74" s="4">
-        <v>75.2</v>
+        <v>95.5</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
@@ -2039,24 +2016,33 @@
         <v>45</v>
       </c>
       <c r="E75" s="3">
-        <v>0.75</v>
+        <v>2</v>
       </c>
       <c r="F75" s="4">
-        <v>80.400000000000006</v>
+        <v>95</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A76" s="12"/>
-      <c r="B76" s="7"/>
-      <c r="C76" s="8"/>
+      <c r="A76" s="11">
+        <v>13</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="D76" s="2">
         <v>45</v>
       </c>
       <c r="E76" s="3">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="F76" s="4">
-        <v>85.3</v>
+        <v>83.17</v>
+      </c>
+      <c r="G76" s="9" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -2064,13 +2050,13 @@
       <c r="B77" s="7"/>
       <c r="C77" s="8"/>
       <c r="D77" s="2">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="E77" s="3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F77" s="4">
-        <v>44.3</v>
+        <v>90.15</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -2078,13 +2064,13 @@
       <c r="B78" s="7"/>
       <c r="C78" s="8"/>
       <c r="D78" s="2">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="E78" s="3">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="F78" s="4">
-        <v>84.9</v>
+        <v>95.51</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -2092,13 +2078,13 @@
       <c r="B79" s="7"/>
       <c r="C79" s="8"/>
       <c r="D79" s="2">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E79" s="3">
         <v>1</v>
       </c>
       <c r="F79" s="4">
-        <v>90.8</v>
+        <v>102.24</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -2106,13 +2092,13 @@
       <c r="B80" s="7"/>
       <c r="C80" s="8"/>
       <c r="D80" s="2">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="E80" s="3">
         <v>1</v>
       </c>
       <c r="F80" s="4">
-        <v>95.5</v>
+        <v>3.81</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
@@ -2120,36 +2106,27 @@
       <c r="B81" s="7"/>
       <c r="C81" s="8"/>
       <c r="D81" s="2">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E81" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F81" s="4">
-        <v>95</v>
+        <v>5.86</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A82" s="11">
-        <v>14</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="A82" s="12"/>
+      <c r="B82" s="7"/>
+      <c r="C82" s="8"/>
       <c r="D82" s="2">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="E82" s="3">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="F82" s="4">
-        <v>83.17</v>
-      </c>
-      <c r="G82" s="9" t="s">
-        <v>39</v>
+        <v>100</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
@@ -2157,13 +2134,13 @@
       <c r="B83" s="7"/>
       <c r="C83" s="8"/>
       <c r="D83" s="2">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="E83" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F83" s="4">
-        <v>90.15</v>
+        <v>97</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
@@ -2174,24 +2151,33 @@
         <v>45</v>
       </c>
       <c r="E84" s="3">
-        <v>0.75</v>
+        <v>2</v>
       </c>
       <c r="F84" s="4">
-        <v>95.51</v>
+        <v>110</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A85" s="12"/>
-      <c r="B85" s="7"/>
-      <c r="C85" s="8"/>
+      <c r="A85" s="11">
+        <v>14</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="D85" s="2">
         <v>45</v>
       </c>
       <c r="E85" s="3">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="F85" s="4">
-        <v>102.24</v>
+        <v>47.6</v>
+      </c>
+      <c r="G85" s="9" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
@@ -2199,13 +2185,13 @@
       <c r="B86" s="7"/>
       <c r="C86" s="8"/>
       <c r="D86" s="2">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="E86" s="3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F86" s="4">
-        <v>3.81</v>
+        <v>52.9</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
@@ -2213,13 +2199,13 @@
       <c r="B87" s="7"/>
       <c r="C87" s="8"/>
       <c r="D87" s="2">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="E87" s="3">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="F87" s="4">
-        <v>5.86</v>
+        <v>72.5</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
@@ -2227,13 +2213,13 @@
       <c r="B88" s="7"/>
       <c r="C88" s="8"/>
       <c r="D88" s="2">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E88" s="3">
         <v>1</v>
       </c>
       <c r="F88" s="4">
-        <v>100</v>
+        <v>83.3</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
@@ -2241,13 +2227,13 @@
       <c r="B89" s="7"/>
       <c r="C89" s="8"/>
       <c r="D89" s="2">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="E89" s="3">
         <v>1</v>
       </c>
       <c r="F89" s="4">
-        <v>97</v>
+        <v>3.17</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
@@ -2255,36 +2241,27 @@
       <c r="B90" s="7"/>
       <c r="C90" s="8"/>
       <c r="D90" s="2">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E90" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F90" s="4">
-        <v>110</v>
+        <v>6.74</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A91" s="11">
-        <v>15</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>16</v>
-      </c>
+      <c r="A91" s="12"/>
+      <c r="B91" s="7"/>
+      <c r="C91" s="8"/>
       <c r="D91" s="2">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="E91" s="3">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="F91" s="4">
-        <v>47.6</v>
-      </c>
-      <c r="G91" s="9" t="s">
-        <v>39</v>
+        <v>82.8</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
@@ -2292,13 +2269,13 @@
       <c r="B92" s="7"/>
       <c r="C92" s="8"/>
       <c r="D92" s="2">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="E92" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F92" s="4">
-        <v>52.9</v>
+        <v>91.5</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
@@ -2309,24 +2286,33 @@
         <v>45</v>
       </c>
       <c r="E93" s="3">
-        <v>0.75</v>
+        <v>2</v>
       </c>
       <c r="F93" s="4">
-        <v>72.5</v>
+        <v>86.6</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A94" s="12"/>
-      <c r="B94" s="7"/>
-      <c r="C94" s="8"/>
+      <c r="A94" s="11">
+        <v>15</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="D94" s="2">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="E94" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F94" s="4">
-        <v>83.3</v>
+        <v>40.4</v>
+      </c>
+      <c r="G94" s="9" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
@@ -2334,13 +2320,13 @@
       <c r="B95" s="7"/>
       <c r="C95" s="8"/>
       <c r="D95" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E95" s="3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F95" s="4">
-        <v>3.17</v>
+        <v>79.400000000000006</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
@@ -2348,13 +2334,13 @@
       <c r="B96" s="7"/>
       <c r="C96" s="8"/>
       <c r="D96" s="2">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="E96" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F96" s="4">
-        <v>6.74</v>
+        <v>93.7</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
@@ -2362,13 +2348,13 @@
       <c r="B97" s="7"/>
       <c r="C97" s="8"/>
       <c r="D97" s="2">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="E97" s="3">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="F97" s="4">
-        <v>82.8</v>
+        <v>100</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
@@ -2376,13 +2362,13 @@
       <c r="B98" s="7"/>
       <c r="C98" s="8"/>
       <c r="D98" s="2">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E98" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F98" s="4">
-        <v>91.5</v>
+        <v>81</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
@@ -2390,50 +2376,50 @@
       <c r="B99" s="7"/>
       <c r="C99" s="8"/>
       <c r="D99" s="2">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="E99" s="3">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F99" s="4">
-        <v>86.6</v>
+        <v>87.4</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A100" s="11">
+      <c r="A100" s="12"/>
+      <c r="B100" s="7"/>
+      <c r="C100" s="8"/>
+      <c r="D100" s="2">
+        <v>60</v>
+      </c>
+      <c r="E100" s="3">
+        <v>24</v>
+      </c>
+      <c r="F100" s="4">
+        <v>101.1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A101" s="11">
         <v>16</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C100" s="6" t="s">
+      <c r="B101" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D100" s="2">
-        <v>26</v>
-      </c>
-      <c r="E100" s="3">
-        <v>6</v>
-      </c>
-      <c r="F100" s="4">
-        <v>40.4</v>
-      </c>
-      <c r="G100" s="9" t="s">
+      <c r="C101" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D101" s="2">
+        <v>25</v>
+      </c>
+      <c r="E101" s="3">
+        <v>3</v>
+      </c>
+      <c r="F101" s="4">
+        <v>0</v>
+      </c>
+      <c r="G101" s="9" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A101" s="12"/>
-      <c r="B101" s="7"/>
-      <c r="C101" s="8"/>
-      <c r="D101" s="2">
-        <v>26</v>
-      </c>
-      <c r="E101" s="3">
-        <v>12</v>
-      </c>
-      <c r="F101" s="4">
-        <v>79.400000000000006</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
@@ -2441,13 +2427,13 @@
       <c r="B102" s="7"/>
       <c r="C102" s="8"/>
       <c r="D102" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E102" s="3">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="F102" s="4">
-        <v>93.7</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
@@ -2455,13 +2441,13 @@
       <c r="B103" s="7"/>
       <c r="C103" s="8"/>
       <c r="D103" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E103" s="3">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="F103" s="4">
-        <v>100</v>
+        <v>8.6</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
@@ -2469,13 +2455,13 @@
       <c r="B104" s="7"/>
       <c r="C104" s="8"/>
       <c r="D104" s="2">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="E104" s="3">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F104" s="4">
-        <v>81</v>
+        <v>71.400000000000006</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
@@ -2483,105 +2469,12 @@
       <c r="B105" s="7"/>
       <c r="C105" s="8"/>
       <c r="D105" s="2">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="E105" s="3">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F105" s="4">
-        <v>87.4</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A106" s="12"/>
-      <c r="B106" s="7"/>
-      <c r="C106" s="8"/>
-      <c r="D106" s="2">
-        <v>60</v>
-      </c>
-      <c r="E106" s="3">
-        <v>24</v>
-      </c>
-      <c r="F106" s="4">
-        <v>101.1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A107" s="11">
-        <v>17</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C107" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D107" s="2">
-        <v>25</v>
-      </c>
-      <c r="E107" s="3">
-        <v>3</v>
-      </c>
-      <c r="F107" s="4">
-        <v>0</v>
-      </c>
-      <c r="G107" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A108" s="12"/>
-      <c r="B108" s="7"/>
-      <c r="C108" s="8"/>
-      <c r="D108" s="2">
-        <v>25</v>
-      </c>
-      <c r="E108" s="3">
-        <v>6</v>
-      </c>
-      <c r="F108" s="4">
-        <v>12.4</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A109" s="12"/>
-      <c r="B109" s="7"/>
-      <c r="C109" s="8"/>
-      <c r="D109" s="2">
-        <v>25</v>
-      </c>
-      <c r="E109" s="3">
-        <v>9</v>
-      </c>
-      <c r="F109" s="4">
-        <v>8.6</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A110" s="12"/>
-      <c r="B110" s="7"/>
-      <c r="C110" s="8"/>
-      <c r="D110" s="2">
-        <v>25</v>
-      </c>
-      <c r="E110" s="3">
-        <v>12</v>
-      </c>
-      <c r="F110" s="4">
-        <v>71.400000000000006</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A111" s="12"/>
-      <c r="B111" s="7"/>
-      <c r="C111" s="8"/>
-      <c r="D111" s="2">
-        <v>25</v>
-      </c>
-      <c r="E111" s="3">
-        <v>24</v>
-      </c>
-      <c r="F111" s="4">
         <v>81.3</v>
       </c>
     </row>

</xml_diff>